<commit_message>
Pārvietošana un mobilizēšanas logs pievienots, izšķirtspējas izlabošana, dokumentāciju labošana°
</commit_message>
<xml_diff>
--- a/Tehniskā dokumentācija/Testēšana Brīvības cīņas.xlsx
+++ b/Tehniskā dokumentācija/Testēšana Brīvības cīņas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LPO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LPO\Documents\BrivibasCinas\Tehniskā dokumentācija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9120E705-273E-4D59-AE16-021378BA1CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6198AB-07F9-4D79-8372-4C5B07E794CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B0C56B42-C5C8-4527-A706-ECAE942110AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0C56B42-C5C8-4527-A706-ECAE942110AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="216">
   <si>
     <t>Idenfikatoru atšifrējums:</t>
   </si>
@@ -532,13 +532,157 @@
   </si>
   <si>
     <t>KZ.LAT.06</t>
+  </si>
+  <si>
+    <t>TZ.B.12.</t>
+  </si>
+  <si>
+    <t>TZ.B.13.</t>
+  </si>
+  <si>
+    <t>TZ.B.14.</t>
+  </si>
+  <si>
+    <t>IZV</t>
+  </si>
+  <si>
+    <t>Izvēle</t>
+  </si>
+  <si>
+    <t>LID</t>
+  </si>
+  <si>
+    <t>Spēles izvēle</t>
+  </si>
+  <si>
+    <t>PR.IZV.01</t>
+  </si>
+  <si>
+    <t>PR.IZV.02</t>
+  </si>
+  <si>
+    <t>PR.IZV.03</t>
+  </si>
+  <si>
+    <t>PR.SAK.04.</t>
+  </si>
+  <si>
+    <t>Spēles ainas ielāde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spēlēt ar botu </t>
+  </si>
+  <si>
+    <t>Spēlēt 1 pret 1</t>
+  </si>
+  <si>
+    <t>Līderu lauks</t>
+  </si>
+  <si>
+    <t>SAG</t>
+  </si>
+  <si>
+    <t>Saglabāt</t>
+  </si>
+  <si>
+    <t>IEP</t>
+  </si>
+  <si>
+    <t>Iepriekšējais progress</t>
+  </si>
+  <si>
+    <t>OTR</t>
+  </si>
+  <si>
+    <t>Otrs lietotājs</t>
+  </si>
+  <si>
+    <t>ATS</t>
+  </si>
+  <si>
+    <t>Atsākt</t>
+  </si>
+  <si>
+    <t>APR</t>
+  </si>
+  <si>
+    <t>Vēsturisks apraksts</t>
+  </si>
+  <si>
+    <t>PAL</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>Rotu palielināšana</t>
+  </si>
+  <si>
+    <t>Rotu samazināšana</t>
+  </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>Rotu atkāpšanās</t>
+  </si>
+  <si>
+    <t>PR.LAT.07.</t>
+  </si>
+  <si>
+    <t>Spēles rotu palielināšana</t>
+  </si>
+  <si>
+    <t>Spēles rotu samazināšana</t>
+  </si>
+  <si>
+    <t>Spēles rotu uzvarēšana</t>
+  </si>
+  <si>
+    <t>Spēles rotu zaudēšana</t>
+  </si>
+  <si>
+    <t>Spēles rotu atkāpšanās</t>
+  </si>
+  <si>
+    <t>Spēles progresu saglabāšana</t>
+  </si>
+  <si>
+    <t>Spēles iepriekšējais progress</t>
+  </si>
+  <si>
+    <t>PR.LAT.08.</t>
+  </si>
+  <si>
+    <t>PR.LAT.09.</t>
+  </si>
+  <si>
+    <t>PR.LAT.10.</t>
+  </si>
+  <si>
+    <t>PR.LAT.11.</t>
+  </si>
+  <si>
+    <t>PR.LAT.12.</t>
+  </si>
+  <si>
+    <t>PR.LAT.13.</t>
+  </si>
+  <si>
+    <t>PR.LAT.14.</t>
+  </si>
+  <si>
+    <t>PR.LAT.15.</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,6 +766,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -673,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -697,6 +849,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -724,7 +877,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,23 +1192,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19930E9-390E-44F3-A281-41A941A5DA96}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="A4:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1064,19 +1217,19 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1095,150 +1248,253 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="13"/>
+      <c r="C13" s="14"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="13"/>
+      <c r="C14" s="14"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="13"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="13"/>
+      <c r="C16" s="14"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="13"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="13"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="13"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C33" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="29">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B21:C21"/>
@@ -1255,9 +1511,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1266,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E44EBC5-0971-4FC8-9842-6658A0759BB0}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,8 +1540,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1329,95 +1582,205 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>63</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="9"/>
-    </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
+      <c r="A14" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="9"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
+      <c r="A18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>129</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B24" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>210</v>
+      </c>
+      <c r="B29" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>211</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>214</v>
+      </c>
+      <c r="B33" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1432,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214DAA82-A5B2-4DC9-AAA1-ECC0BC576048}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,16 +1838,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1513,14 +1876,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1549,14 +1912,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1585,14 +1948,14 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1621,14 +1984,14 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
@@ -1657,14 +2020,14 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1693,14 +2056,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1729,14 +2092,14 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1765,14 +2128,14 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1870,10 +2233,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80724A93-B008-4A33-8DA6-F5EB9092A099}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,16 +2278,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1947,14 +2310,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1977,14 +2340,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2007,14 +2370,14 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2037,14 +2400,14 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2067,14 +2430,14 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2092,7 +2455,7 @@
       <c r="E13" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="13" t="s">
         <v>138</v>
       </c>
       <c r="G13" t="s">
@@ -2103,14 +2466,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2128,7 +2491,7 @@
       <c r="E15" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="13" t="s">
         <v>138</v>
       </c>
       <c r="G15" t="s">
@@ -2139,16 +2502,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>137</v>
       </c>
@@ -2168,17 +2531,17 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>163</v>
       </c>
@@ -2198,7 +2561,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>165</v>
       </c>
@@ -2217,8 +2580,11 @@
       <c r="F20" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>164</v>
       </c>
@@ -2234,7 +2600,7 @@
       <c r="E21" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="13" t="s">
         <v>138</v>
       </c>
       <c r="G21" t="s">
@@ -2244,28 +2610,110 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="11">
+        <v>45446</v>
+      </c>
+      <c r="C23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B25" s="11">
+        <v>45446</v>
+      </c>
+      <c r="C25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="11">
+        <v>45446</v>
+      </c>
+      <c r="C26" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A10:H10"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
25 testpiemēri, dokumentāciju labošana/pievienošana
</commit_message>
<xml_diff>
--- a/Tehniskā dokumentācija/Testēšana Brīvības cīņas.xlsx
+++ b/Tehniskā dokumentācija/Testēšana Brīvības cīņas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LPO\Documents\BrivibasCinas\Tehniskā dokumentācija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6198AB-07F9-4D79-8372-4C5B07E794CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE19061A-FE42-48AB-A776-B72DE3498B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0C56B42-C5C8-4527-A706-ECAE942110AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B0C56B42-C5C8-4527-A706-ECAE942110AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="397">
   <si>
     <t>Idenfikatoru atšifrējums:</t>
   </si>
@@ -237,9 +237,6 @@
     <t>PR.LAT.01.</t>
   </si>
   <si>
-    <t>Spēles rotu kustināšana</t>
-  </si>
-  <si>
     <t>Spēles rotu mobilizēšana</t>
   </si>
   <si>
@@ -345,9 +342,6 @@
     <t>1)Jābut startētai datorspēlei "Brīvibas cīņas" 2) Jābūt atvērtai iestatījuma ainai</t>
   </si>
   <si>
-    <t xml:space="preserve">Jebkuras izšķirtspējas nomaiņa </t>
-  </si>
-  <si>
     <t>1)Jābūt nospietam dropdown, kur parādās izsķirtspēja 2)Izvēlās jebkuru izšķirtspēja, kura nav tā pati</t>
   </si>
   <si>
@@ -369,15 +363,9 @@
     <t>Spēles skaņas efektu sviras pavilkšana uz jebkuru pusi - vai klusāk vai skaļāk</t>
   </si>
   <si>
-    <t>1)Jābūt nospietam dropdown, kur parādās izsķirtspēja 2)Pavelk mūzikas apjoma sviru uz jebkuru pusi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Peles kreisā taustiņa klikšķis un jāvelk </t>
   </si>
   <si>
-    <t>1)Jābūt nospietam dropdown, kur parādās izsķirtspēja 2)Pavelk skaņas efekta apjoma sviru uz jebkuru pusi</t>
-  </si>
-  <si>
     <t>Mūzikas skaļums mainās</t>
   </si>
   <si>
@@ -676,13 +664,599 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>PR.LAT.07</t>
+  </si>
+  <si>
+    <t>PR.LAT.08</t>
+  </si>
+  <si>
+    <t>Lietotāja uzbrukšanas rotu palielināšana</t>
+  </si>
+  <si>
+    <t>PR.LAT.UZB.PAL.04</t>
+  </si>
+  <si>
+    <t>Lietotāja uzbrukšanas rotu samazināšana</t>
+  </si>
+  <si>
+    <t>Lietotāju rotu uzbrukšanas palielināšana ar + pogu</t>
+  </si>
+  <si>
+    <t>1)Jānospiež poga "+"</t>
+  </si>
+  <si>
+    <t>Skaits palielinās</t>
+  </si>
+  <si>
+    <t>Skaits samazinās</t>
+  </si>
+  <si>
+    <t>1)Jānospiež poga "-"</t>
+  </si>
+  <si>
+    <t>Lietotāju rotu uzbrukšanas samazināšana ar - pogu</t>
+  </si>
+  <si>
+    <t>Spēles rotu pārvietošana</t>
+  </si>
+  <si>
+    <t>Lietotāja pārvietošana uz blakus teritoriju iekrāsošana</t>
+  </si>
+  <si>
+    <t>1)Jābūt noklikšķinātam uz jebkuru savu teritoriju 2)Jānospiež poga "Pārvietot"</t>
+  </si>
+  <si>
+    <t>Lietotāja uzbrukšana blakus teritorijām iekrāsošana, kad nospiež pogu "Pārvietot"</t>
+  </si>
+  <si>
+    <t>1)Jānospiež poga "Pārvietot"</t>
+  </si>
+  <si>
+    <t>Iekrāsojās tuvākie pārvietošanās lauki</t>
+  </si>
+  <si>
+    <t>PR.LAT.04</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAR.01</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAR.02</t>
+  </si>
+  <si>
+    <t>Lietotāja pārvietošana uz blakus teritoriju ieklikšķināšana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Jābūt noklikšķinātam uz jebkuru savu blakus iekrāsoto teritoriju </t>
+  </si>
+  <si>
+    <t>Lietotāja pārvietošana blakus sava teritorija noklikšķināšana, lai parādās lauks ar cik rotām pārvietoties</t>
+  </si>
+  <si>
+    <t>Parādās lauks ar cik rotām pārvietoties</t>
+  </si>
+  <si>
+    <t>PR.LAT.UZB.SAM.05</t>
+  </si>
+  <si>
+    <t>Lietotāja pārvietošana rotu palielināšana</t>
+  </si>
+  <si>
+    <t>Lietotāja pārvietošana rotu samazināšana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Jābūt noklikšķinātam uz jebkuru lietotāju teritoriju </t>
+  </si>
+  <si>
+    <t>Lietotāju rotu pārvietošanas palielināšana ar + pogu</t>
+  </si>
+  <si>
+    <t>Lietotāju rotu pārvietošanas samazināšana ar - pogu</t>
+  </si>
+  <si>
+    <t>Lietotāja mobilizēšana savā teritorijā</t>
+  </si>
+  <si>
+    <t>PR.LAT.MOB.01</t>
+  </si>
+  <si>
+    <t>1)Jābūt noklikšķinātam uz jebkuru savu teritoriju 2)Jānospiež poga "Mobilizēt"</t>
+  </si>
+  <si>
+    <t>Lietotāja mobilizēšanas lauks ar skaitu, cik daudz mobilizēt</t>
+  </si>
+  <si>
+    <t>1)Jānospiež poga "Mobilizēt"</t>
+  </si>
+  <si>
+    <t>Parādās lauks cik rotas mobilizēt</t>
+  </si>
+  <si>
+    <t>Lietotāja mobilizēšana rotu palielināšana</t>
+  </si>
+  <si>
+    <t>Lietotāja mobilizēšana rotu samazināšana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Jābūt noklikšķinātam uz jebkuru lietotāju teritoriju 2)Jābut nospiestai pogai "Mobilizēt" </t>
+  </si>
+  <si>
+    <t>PR.LAT.MOB.PAL.02</t>
+  </si>
+  <si>
+    <t>PR.LAT.MOB.SAM.03</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAR.PAL.03</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAR.SAM.04</t>
+  </si>
+  <si>
+    <t>PR.LAT.MOB.04</t>
+  </si>
+  <si>
+    <t>Mobilizēt rotas Lietotāja teritorijā</t>
+  </si>
+  <si>
+    <t>1)Jābūt noklikšķinātam uz jebkuru lietotāju teritoriju 2)Jābut nospiestai pogai "Mobilizēt" 3)Izvēlās rotas skaitu cik grib mobilizēt atkarībā no dotā mobilizēšanas skaita</t>
+  </si>
+  <si>
+    <t>Lietotāju rotu mobilizēšanas samazināšana ar - pogu</t>
+  </si>
+  <si>
+    <t>Lietotāju rotu mobilizēšanas palielināšana ar + pogu</t>
+  </si>
+  <si>
+    <t>Lietotāju rotu mobilizēšanas samazināšana ar "OK" pogu</t>
+  </si>
+  <si>
+    <t>1)Jānospiež poga "OK"</t>
+  </si>
+  <si>
+    <t>1)Jaunas rotas mobilizējās teritorijā 2)Parādās ziņojums, ka ir mobilizētas jaunas rotas</t>
+  </si>
+  <si>
+    <t>PAU</t>
+  </si>
+  <si>
+    <t>Pauze</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAU.01</t>
+  </si>
+  <si>
+    <t>Spēles pauze</t>
+  </si>
+  <si>
+    <t>Spēles nopauzēšana ar ESC pogu</t>
+  </si>
+  <si>
+    <t>1)Jānospiež taustiņš "ESC"</t>
+  </si>
+  <si>
+    <t>Taustiņš "ESC"</t>
+  </si>
+  <si>
+    <t>1)Fons paliek pelēks 2)Parādās jaunas opcijas</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAU.AUD.02</t>
+  </si>
+  <si>
+    <t>1)Jābūt atvērtai ESC izvēlnei</t>
+  </si>
+  <si>
+    <t>1)Pavelk mūzikas apjoma sviru uz jebkuru pusi</t>
+  </si>
+  <si>
+    <t>1)Pavelk skaņas efekta apjoma sviru uz jebkuru pusi</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAU.AUD.03</t>
+  </si>
+  <si>
+    <t>Spēles mūzikas skaļuma regulēšana pauzes laikā</t>
+  </si>
+  <si>
+    <t>Spēles efektu skaļuma regulēšana pauzes laikā</t>
+  </si>
+  <si>
+    <t>Spēles efektu sviras pavilkšana uz jebkuru pusi - vai klusāk vai skaļāk</t>
+  </si>
+  <si>
+    <t>1)Pavelk efektu skaļumu sviru uz jebkuru pusi</t>
+  </si>
+  <si>
+    <t>1)Pavelk mūzikas skaļumu sviru uz jebkuru pusi</t>
+  </si>
+  <si>
+    <t>Efekta skaļums mainās</t>
+  </si>
+  <si>
+    <t>SAI</t>
+  </si>
+  <si>
+    <t>Sākuma ainas ielāde</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAU.SAI.04</t>
+  </si>
+  <si>
+    <t>Atgriezšanās uz sākuma aina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Jābūt atvērtai ESC izvēlnei </t>
+  </si>
+  <si>
+    <t>Spēles pogu "Iziet" noklikšķināšana uz sākuma ainu</t>
+  </si>
+  <si>
+    <t>1)Ar peles kreiso kliķšķi jānospiež poga "Iziet"</t>
+  </si>
+  <si>
+    <t>Atgriežanās uz sākuma ainu</t>
+  </si>
+  <si>
+    <t>1)Jānoklikšķina jebkura blakus iekrāsotā teritorija</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAU.KAI.04</t>
+  </si>
+  <si>
+    <t>Sākt spēli no jauna</t>
+  </si>
+  <si>
+    <t>Spēles pogu "Sākt no jauna" noklikšķināšana uz sākuma ainu</t>
+  </si>
+  <si>
+    <t>1)Ar peles kreiso kliķšķi jānospiež poga "Sākt no jauna"</t>
+  </si>
+  <si>
+    <t>Spēle sākās no jauna</t>
+  </si>
+  <si>
+    <t>PR.LAT.16.</t>
+  </si>
+  <si>
+    <t>Spēle sākšana no jauna</t>
+  </si>
+  <si>
+    <t>PR.LAT.APR.01.</t>
+  </si>
+  <si>
+    <t>Spēles vēsturiskais apraksts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vēsturiskais apraksts, kad ir ieņemta lielāka pilsēta </t>
+  </si>
+  <si>
+    <t>1)Noklikšķināt uz savu teritoriju 2)Nospiest pogu "Uzbrukt" 3)Izvēlēties uzbrukt pilsētai 4)Uzbrukt ar rotas skaitu ar kādu var uzvarēt</t>
+  </si>
+  <si>
+    <t>Parādīsies vēsturiskais apraksts</t>
+  </si>
+  <si>
+    <t>PR.LAT.17.</t>
+  </si>
+  <si>
+    <t>1)Jābūt uzbruktai pretinieku teritorijā</t>
+  </si>
+  <si>
+    <t>PR.LAT.UZV.01</t>
+  </si>
+  <si>
+    <t>Spēles uzvarēšana kā Latvija</t>
+  </si>
+  <si>
+    <t>1)Iebrukt pretinieku teritorijā tik daudz, līdz kamēr paliek 5 teritorijas</t>
+  </si>
+  <si>
+    <t>1)Fons paliek pelēks 2)Parādās lauks, ka Latvija ir uzvarējusi</t>
+  </si>
+  <si>
+    <t>PR.LAT.18.</t>
+  </si>
+  <si>
+    <t>PR.LAT.19.</t>
+  </si>
+  <si>
+    <t>Spēles uzvarēšana</t>
+  </si>
+  <si>
+    <t>Spēles zaudēšana</t>
+  </si>
+  <si>
+    <t>PR.LAT.UZV.02</t>
+  </si>
+  <si>
+    <t>Spēles uzvarēšana kā LSPR</t>
+  </si>
+  <si>
+    <t>1)Iebrukt pretinieku teritorijā tik daudz, līdz kamēr paliek 1 teritorijas</t>
+  </si>
+  <si>
+    <t>1)Fons paliek pelēks 2)Parādās lauks, ka lielinieki ir uzvarējuši un Latvija padodas</t>
+  </si>
+  <si>
+    <t>PR.LAT.ZAU.01</t>
+  </si>
+  <si>
+    <t>1)Jābūt izvēlētam AI spēles veids 2)Jābut, ka Latvijas teritorijā ir atlikušas tikai 1 vietas, kur iebrukt</t>
+  </si>
+  <si>
+    <t>1)Jābūt izvēlētam 1 pret 1 spēles veids 2)Jābut, ka Latvijas teritorijā ir atlikušas tikai 1 vietas, kur iebrukt</t>
+  </si>
+  <si>
+    <t>Spēle zaudēšana kā lietotājs</t>
+  </si>
+  <si>
+    <t>1)Jābut, ka pretinieku teritorijā ir atlikušas tikai 5 vietas, kur iebrukt 2)Var būt jebkura spēles izvēle</t>
+  </si>
+  <si>
+    <t>AI izdarītais gājiens</t>
+  </si>
+  <si>
+    <t>White box</t>
+  </si>
+  <si>
+    <t>PR.LAT.PAU.ATS.04</t>
+  </si>
+  <si>
+    <t>Atsākt spēli</t>
+  </si>
+  <si>
+    <t>1)Jānospiež taustiņš ESC</t>
+  </si>
+  <si>
+    <t>Spēles atsākšana ar ESC pogu</t>
+  </si>
+  <si>
+    <t>Jebkuras izšķirtspējas nomaiņa ar kreiso peles klikšķī</t>
+  </si>
+  <si>
+    <t>PR.IZV.POG.01</t>
+  </si>
+  <si>
+    <t>PR.IZV.POG.02</t>
+  </si>
+  <si>
+    <t>Spēles izvēle uz 1 pret 1</t>
+  </si>
+  <si>
+    <t>Spēles izvēle pret botu</t>
+  </si>
+  <si>
+    <t>PR.IZV.POG.03</t>
+  </si>
+  <si>
+    <t>Unity izstrādes vidē ir jābūt atvērtam spēles izvēles ainai</t>
+  </si>
+  <si>
+    <t>Peles kreiso klikšķi uz 1 pret 1 pogu</t>
+  </si>
+  <si>
+    <t>Peles kreiso klikšķi uz spēlet ar botu pogu</t>
+  </si>
+  <si>
+    <t>Peles kreiso klikšķi uz atpakaļ pogu</t>
+  </si>
+  <si>
+    <t>1)Ar peles kreiso klikšķi nospiest pogu "Spēlet 1 pret 1"</t>
+  </si>
+  <si>
+    <t>1)Ar peles kreiso klikšķi nospiest pogu "Spēlet ar botu"</t>
+  </si>
+  <si>
+    <t>1)Ar peles kreiso klikšķi nospiest pogu "Atpakaļ"</t>
+  </si>
+  <si>
+    <t>1)Ar onclick.Addlistener tiek padoda informācija ka ir nospiesta SpēlesIzvēle bez AI 
+2)Ieiet SpelesIzvele funkcijā un padod informāciju PlayerPrefs.setInt("Grutiba", izveletaPoga)
+ 3)Ar SceneManager ielādējas Spēles aina
+4)Void Awake() funkcijā dabū informāciju par spēles izvēles veidu</t>
+  </si>
+  <si>
+    <t>1)Ar onclick.Addlistener tiek padoda informācija ka ir nospiesta SpēlesIzvēle ar AI 
+2)Ieiet SpelesIzvele funkcijā un padod informāciju PlayerPrefs.setInt("Grutiba", izveletaPoga)
+ 3)Ar SceneManager ielādējas Spēles aina
+4)Void Awake() funkcijā dabū informāciju par spēles izvēles veidu</t>
+  </si>
+  <si>
+    <t>1)Ar SceneManager ielādējas galvenā aina</t>
+  </si>
+  <si>
+    <t>Lietotāja uzbrukšanas uzvarēšana</t>
+  </si>
+  <si>
+    <t>1)Ar peles kreiso klikšķi uzspiest "OK" pogu.</t>
+  </si>
+  <si>
+    <t>Lietotāja uzbrukšanas zaudēšana</t>
+  </si>
+  <si>
+    <t>1)Funkcija pārbaudīs, ja objekti.rotuSkaitsIzv&gt; StateController.rotasSkaitsByPlayer[Valsts.Speletaji.LSPR
+2)Pretinieks/Spēlētājs atkāpsies uz tukšāko teritoriju, ja nav tukšākās, tad atkāpsies uz teritoriju, kur ir rotas, ja nav nekur kur atkāpties, tad irIelenktas = true, kas nozimē, ka ir ielenktas
+3)Ar for ciklu izdzesīs vecās rotas, izmantotās pozīcijas un iedos ka iruzbrucis = true
+4)Pados teksts.vesturisksNotikums(), kur parādīsies, ka ir uzbrucis un skatīsies, vai ir ieņēmis svarīgu pilsētu
+5)Pievienos Uzbrukušās rotas ar nākamo for ciklu uz jauno teritoriju
+6)Parādīsies ziņojums, ka ir uzvarējis cīņu</t>
+  </si>
+  <si>
+    <t>Lietotāju pārvietošanās pa savu teritoriju</t>
+  </si>
+  <si>
+    <t>1)Izvēlēties savu teritoriju, kurā ir rotas
+2)Jāizvēlas poga "Uzbrukt"
+3)Jābut uzsķlikšķinātai jebkurai blakus pretinieku teritorijai
+4)Jābūt rotu pārsvars, lai uzvarētu</t>
+  </si>
+  <si>
+    <t>1)Izvēlēties savu teritoriju, kurā ir rotas
+2)Jāizvēlas poga "Uzbrukt"
+3)Jābut uzsķlikšķinātai jebkurai blakus pretinieku teritorijai
+4)Jābūt rotu mazākums, lai zaudētu</t>
+  </si>
+  <si>
+    <t>1)Izvēlēties savu teritoriju, kurā ir rotas
+2)Jāizvēlas poga "Pārvietot"
+3)Jābut uzsķlikšķinātai jebkurai lietotāju teritorijai, kurā nav 5 rotas
+4)Izvēlās vismaz 1 rotu pārvietošanai</t>
+  </si>
+  <si>
+    <t>Ar peles kreiso klikšķi uz "OK" pogu, lai zaudētu</t>
+  </si>
+  <si>
+    <t>Ar peles kreiso klikšķi uz "OK" pogu, lai uzvarētu</t>
+  </si>
+  <si>
+    <t>Ar peles kreiso klikšķi uz "OK" pogu, lai pārvietotu rotas</t>
+  </si>
+  <si>
+    <t>1)Funkcijā sākumā ar for ciklu pārvietos pārvietotās rotas un pārvietoto teritoriju un saskaita pārvietojumo skaitu
+2)Otrā for ciklā izdzēš rotu no iepriekšējas teritorijas
+3)Parādās ziņojums, ka ir pārvietojusies rota</t>
+  </si>
+  <si>
+    <t>PAR.LAT.AI.01</t>
+  </si>
+  <si>
+    <t>AI uzbrukšana uz vājāko vietu</t>
+  </si>
+  <si>
+    <t>Pēc lietotāja izdarītas gaitas AI uzbruks lietotāja vājāka vietā</t>
+  </si>
+  <si>
+    <t>1)Jābūt izvēlētai spēlet ar botu
+2)Lietotājam sākuma ir jāizdara gaita, jāuzbrūk, lai ir tukša teritorija
+3)Lietotājam ir jānospiež "OK" poga pēc izdarītā gaita.</t>
+  </si>
+  <si>
+    <t>1)Pēc lietotāja izdarītās gaitas</t>
+  </si>
+  <si>
+    <t>Pēc lietotāja izdarītās gaitas</t>
+  </si>
+  <si>
+    <t>1)AI saņem informāciju, ka ir jādara AIKustiba, kur prioritāte it LSPRUzbrukums();
+2)LSPRUzbrukums(), dabū State, no kura tiks darītas gaitas
+3)Tagad meklē ar distance &lt; 1.96f, tuvākās lietotāja teritorijas, kur stateControllerrotasSkaitsByPlayer[Valstis.Speletaji.PLAYER] &lt; objekti.noKuraStateLSPRKontrole.rotasSkaitsByPlayer[Valstis.Speletaji.LSPR]
+4)Ja ir atrasts UzbruksanasState, tad uzbrūk lietotājam un ieņem teritoriju.
+5)Lietotājs atkāpsies uz tukšāko teritoriju, ja nav tukšākās, tad atkāpsies uz teritoriju, kur ir rotas, ja nav nekur kur atkāpties, tad irIelenktas = true, kas nozimē, ka ir ielenktas
+6)Tad ar for ciklu pievieno jaunās pretinieku rotas iekarotā teritorijā
+7)Ar otru ciklu izdzēšs ārā vecās LSPR(AI) rotas teritorijā</t>
+  </si>
+  <si>
+    <t>PR.LAT.20.</t>
+  </si>
+  <si>
+    <t>PR.LAT.21.</t>
+  </si>
+  <si>
+    <t>PR.LAT.22.</t>
+  </si>
+  <si>
+    <t>Spēles AI uzbrukšana</t>
+  </si>
+  <si>
+    <t>Spēles AI mobilizēšana</t>
+  </si>
+  <si>
+    <t>Spēles AI atkāpšanās</t>
+  </si>
+  <si>
+    <t>1)Funkcija pārbaudīs, ja objekti.rotuSkaitsIzv &lt; StateController.rotasSkaitsByPlayer[Valsts.Speletaji.LSPR, tad irZaudets = true
+6)Parādīsies ziņojums, ka ir zaudējis cīņu</t>
+  </si>
+  <si>
+    <t>TZ.B.15.</t>
+  </si>
+  <si>
+    <t>TZ.B.16.</t>
+  </si>
+  <si>
+    <t>TZ.B.17.</t>
+  </si>
+  <si>
+    <t>TZ.B.18.</t>
+  </si>
+  <si>
+    <t>TZ.B.19.</t>
+  </si>
+  <si>
+    <t>TZ.B.20.</t>
+  </si>
+  <si>
+    <t>TZ.B.21.</t>
+  </si>
+  <si>
+    <t>TZ.B.22.</t>
+  </si>
+  <si>
+    <t>TZ.B.23.</t>
+  </si>
+  <si>
+    <t>TZ.B.24.</t>
+  </si>
+  <si>
+    <t>TZ.B.25.</t>
+  </si>
+  <si>
+    <t>TZ.B.26.</t>
+  </si>
+  <si>
+    <t>TZ.B.27.</t>
+  </si>
+  <si>
+    <t>TZ.B.28.</t>
+  </si>
+  <si>
+    <t>TZ.B.29.</t>
+  </si>
+  <si>
+    <t>TZ.B.30.</t>
+  </si>
+  <si>
+    <t>TZ.B.31.</t>
+  </si>
+  <si>
+    <t>TZ.B.32.</t>
+  </si>
+  <si>
+    <t>TZ.B.33.</t>
+  </si>
+  <si>
+    <t>TZ.B.34.</t>
+  </si>
+  <si>
+    <t>TZ.W.1.</t>
+  </si>
+  <si>
+    <t>TZ.W.2.</t>
+  </si>
+  <si>
+    <t>TZ.W.3.</t>
+  </si>
+  <si>
+    <t>TZ.W.4.</t>
+  </si>
+  <si>
+    <t>TZ.W.5.</t>
+  </si>
+  <si>
+    <t>TZ.W.6.</t>
+  </si>
+  <si>
+    <t>TZ.W.7.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,8 +1348,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -812,6 +1392,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -825,7 +1411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -850,6 +1436,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -877,7 +1467,12 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1192,23 +1787,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19930E9-390E-44F3-A281-41A941A5DA96}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B33" sqref="A4:C33"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1217,19 +1812,19 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1248,240 +1843,264 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="14"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="14"/>
+        <v>116</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="14"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C23" s="14"/>
+        <v>119</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="14"/>
+        <v>167</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="C25" s="14"/>
+      <c r="A25" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C26" s="14"/>
+        <v>179</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="14"/>
+        <v>181</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="C28" s="14"/>
+        <v>183</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="C29" s="14"/>
+        <v>185</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="C30" s="14"/>
+        <v>187</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="C31" s="14"/>
+        <v>189</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C32" s="14"/>
+        <v>190</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="C33" s="14"/>
+        <v>193</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" s="16"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="C34" s="16"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="32">
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B33:C33"/>
@@ -1496,6 +2115,9 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B11:C11"/>
@@ -1509,7 +2131,6 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1519,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E44EBC5-0971-4FC8-9842-6658A0759BB0}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,8 +2161,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1583,10 +2204,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1629,29 +2250,29 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B14" s="9"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
         <v>65</v>
@@ -1684,76 +2305,76 @@
         <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B25" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B26" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B28" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B29" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B30" t="s">
         <v>61</v>
@@ -1761,7 +2382,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
@@ -1769,18 +2390,74 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B32" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B33" t="s">
-        <v>206</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>296</v>
+      </c>
+      <c r="B34" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>303</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>309</v>
+      </c>
+      <c r="B36" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>310</v>
+      </c>
+      <c r="B37" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>363</v>
+      </c>
+      <c r="B38" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>364</v>
+      </c>
+      <c r="B39" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>365</v>
+      </c>
+      <c r="B40" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -1793,21 +2470,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214DAA82-A5B2-4DC9-AAA1-ECC0BC576048}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1838,385 +2515,1192 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="H3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>88</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>89</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-    </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>95</v>
-      </c>
       <c r="F7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>97</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:8" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="F11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:8" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+    </row>
+    <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>230</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>253</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>254</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+    </row>
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>243</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="H30" t="s">
+        <v>124</v>
+      </c>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>251</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>252</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>255</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="H33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>265</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>271</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-    </row>
-    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>141</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="H36" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>275</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="H37" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>284</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="H38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>291</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="H39" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>324</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="H40" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+    </row>
+    <row r="42" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>298</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="H42" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+    </row>
+    <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>305</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="H44" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>313</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H45" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+    </row>
+    <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>317</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="F47" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H47" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+    </row>
+    <row r="49" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>329</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="H49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>330</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="H50" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>333</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G51" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="H51" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+    </row>
+    <row r="53" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="H53" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>144</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>155</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>147</v>
+      <c r="B54" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G54" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="H54" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+    </row>
+    <row r="56" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>230</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>354</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G56" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="H56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+    </row>
+    <row r="58" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>356</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="F58" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="H58" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="14">
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A48:H48"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A18:H18"/>
@@ -2226,17 +3710,21 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A34:H34"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80724A93-B008-4A33-8DA6-F5EB9092A099}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,430 +3766,1082 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="11">
         <v>45404</v>
       </c>
       <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="11">
         <v>45404</v>
       </c>
       <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="D5" t="s">
-        <v>85</v>
-      </c>
       <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="11">
         <v>45406</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="11">
         <v>45406</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="11">
         <v>45407</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>103</v>
-      </c>
       <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B13" s="11">
         <v>45408</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B15" s="11">
         <v>45408</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B17" s="11">
         <v>45408</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B19" s="11">
         <v>45408</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B20" s="11">
         <v>45408</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="I20" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B21" s="11">
         <v>45408</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G21" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H21" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B23" s="11">
         <v>45446</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B25" s="11">
         <v>45446</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>62</v>
       </c>
       <c r="E25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B26" s="11">
         <v>45446</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>370</v>
+      </c>
+      <c r="B28" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>371</v>
+      </c>
+      <c r="B29" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>372</v>
+      </c>
+      <c r="B31" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C31" t="s">
+        <v>230</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>373</v>
+      </c>
+      <c r="B32" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C32" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E32" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>374</v>
+      </c>
+      <c r="B33" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C33" t="s">
+        <v>253</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E33" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>375</v>
+      </c>
+      <c r="B34" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C34" t="s">
+        <v>254</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>376</v>
+      </c>
+      <c r="B36" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C36" t="s">
+        <v>243</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="E36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>377</v>
+      </c>
+      <c r="B37" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C37" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>378</v>
+      </c>
+      <c r="B38" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C38" t="s">
+        <v>252</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="E38" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>379</v>
+      </c>
+      <c r="B39" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C39" t="s">
+        <v>255</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="E39" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>380</v>
+      </c>
+      <c r="B41" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C41" t="s">
+        <v>265</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>381</v>
+      </c>
+      <c r="B42" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C42" t="s">
+        <v>271</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>382</v>
+      </c>
+      <c r="B43" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C43" t="s">
+        <v>275</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="E43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>383</v>
+      </c>
+      <c r="B44" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C44" t="s">
+        <v>284</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="E44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>384</v>
+      </c>
+      <c r="B45" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C45" t="s">
+        <v>291</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="E45" t="s">
+        <v>81</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>385</v>
+      </c>
+      <c r="B46" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C46" t="s">
+        <v>324</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="E46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>386</v>
+      </c>
+      <c r="B48" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C48" t="s">
+        <v>298</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="E48" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="24"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>387</v>
+      </c>
+      <c r="B50" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C50" t="s">
+        <v>305</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="E50" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>388</v>
+      </c>
+      <c r="B51" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C51" t="s">
+        <v>313</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="E51" t="s">
+        <v>81</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="24"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="24"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>389</v>
+      </c>
+      <c r="B53" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C53" t="s">
+        <v>317</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="E53" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>390</v>
+      </c>
+      <c r="B55" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C55" t="s">
+        <v>329</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="E55" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>391</v>
+      </c>
+      <c r="B56" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C56" t="s">
+        <v>330</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="E56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>392</v>
+      </c>
+      <c r="B57" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C57" t="s">
+        <v>333</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E57" t="s">
+        <v>81</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="24"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+    </row>
+    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>393</v>
+      </c>
+      <c r="B59" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C59" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="E59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>394</v>
+      </c>
+      <c r="B60" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C60" t="s">
+        <v>144</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="E60" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="24"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+    </row>
+    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>395</v>
+      </c>
+      <c r="B62" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C62" t="s">
+        <v>230</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="E62" t="s">
+        <v>81</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="24"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>396</v>
+      </c>
+      <c r="B64" s="11">
+        <v>45447</v>
+      </c>
+      <c r="C64" t="s">
+        <v>356</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="E64" t="s">
+        <v>81</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="22">
+    <mergeCell ref="A52:H52"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="A58:H58"/>
+    <mergeCell ref="A61:H61"/>
+    <mergeCell ref="A63:H63"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A49:H49"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A2:H2"/>

</xml_diff>

<commit_message>
Dokumentāciju labošana - diagrammas, pielikti pielikumi
</commit_message>
<xml_diff>
--- a/Tehniskā dokumentācija/Testēšana Brīvības cīņas.xlsx
+++ b/Tehniskā dokumentācija/Testēšana Brīvības cīņas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LPO\Documents\BrivibasCinas\Tehniskā dokumentācija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE19061A-FE42-48AB-A776-B72DE3498B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50540FB6-0D26-4A81-B865-2A6078EC1FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B0C56B42-C5C8-4527-A706-ECAE942110AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B0C56B42-C5C8-4527-A706-ECAE942110AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="427">
   <si>
     <t>Idenfikatoru atšifrējums:</t>
   </si>
@@ -1120,9 +1120,6 @@
 3)Parādās ziņojums, ka ir pārvietojusies rota</t>
   </si>
   <si>
-    <t>PAR.LAT.AI.01</t>
-  </si>
-  <si>
     <t>AI uzbrukšana uz vājāko vietu</t>
   </si>
   <si>
@@ -1140,7 +1137,202 @@
     <t>Pēc lietotāja izdarītās gaitas</t>
   </si>
   <si>
-    <t>1)AI saņem informāciju, ka ir jādara AIKustiba, kur prioritāte it LSPRUzbrukums();
+    <t>PR.LAT.20.</t>
+  </si>
+  <si>
+    <t>PR.LAT.21.</t>
+  </si>
+  <si>
+    <t>PR.LAT.22.</t>
+  </si>
+  <si>
+    <t>Spēles AI uzbrukšana</t>
+  </si>
+  <si>
+    <t>Spēles AI mobilizēšana</t>
+  </si>
+  <si>
+    <t>Spēles AI atkāpšanās</t>
+  </si>
+  <si>
+    <t>1)Funkcija pārbaudīs, ja objekti.rotuSkaitsIzv &lt; StateController.rotasSkaitsByPlayer[Valsts.Speletaji.LSPR, tad irZaudets = true
+6)Parādīsies ziņojums, ka ir zaudējis cīņu</t>
+  </si>
+  <si>
+    <t>TZ.B.15.</t>
+  </si>
+  <si>
+    <t>TZ.B.16.</t>
+  </si>
+  <si>
+    <t>TZ.B.17.</t>
+  </si>
+  <si>
+    <t>TZ.B.18.</t>
+  </si>
+  <si>
+    <t>TZ.B.19.</t>
+  </si>
+  <si>
+    <t>TZ.B.20.</t>
+  </si>
+  <si>
+    <t>TZ.B.21.</t>
+  </si>
+  <si>
+    <t>TZ.B.22.</t>
+  </si>
+  <si>
+    <t>TZ.B.23.</t>
+  </si>
+  <si>
+    <t>TZ.B.24.</t>
+  </si>
+  <si>
+    <t>TZ.B.25.</t>
+  </si>
+  <si>
+    <t>TZ.B.26.</t>
+  </si>
+  <si>
+    <t>TZ.B.27.</t>
+  </si>
+  <si>
+    <t>TZ.B.28.</t>
+  </si>
+  <si>
+    <t>TZ.B.29.</t>
+  </si>
+  <si>
+    <t>TZ.B.30.</t>
+  </si>
+  <si>
+    <t>TZ.B.31.</t>
+  </si>
+  <si>
+    <t>TZ.B.32.</t>
+  </si>
+  <si>
+    <t>TZ.B.33.</t>
+  </si>
+  <si>
+    <t>TZ.B.34.</t>
+  </si>
+  <si>
+    <t>TZ.W.1.</t>
+  </si>
+  <si>
+    <t>TZ.W.2.</t>
+  </si>
+  <si>
+    <t>TZ.W.3.</t>
+  </si>
+  <si>
+    <t>TZ.W.4.</t>
+  </si>
+  <si>
+    <t>TZ.W.5.</t>
+  </si>
+  <si>
+    <t>TZ.W.6.</t>
+  </si>
+  <si>
+    <t>TZ.W.7.</t>
+  </si>
+  <si>
+    <t>AI mobilizēšana tukšākā vietā</t>
+  </si>
+  <si>
+    <t>AI atkāpšanās tukšā teritorijā</t>
+  </si>
+  <si>
+    <t>AI atkāpšanās teritorijā, kur ir rotas</t>
+  </si>
+  <si>
+    <t>PR.LAT.AI.01</t>
+  </si>
+  <si>
+    <t>PR.LAT.AI.02</t>
+  </si>
+  <si>
+    <t>PR.LAT.AI.03</t>
+  </si>
+  <si>
+    <t>PR.LAT.AI.04</t>
+  </si>
+  <si>
+    <t>PR.LAT.LID.01</t>
+  </si>
+  <si>
+    <t>PR.LAT.SAG.01</t>
+  </si>
+  <si>
+    <t>PR.LAT.SAG.02</t>
+  </si>
+  <si>
+    <t>PR.LAT.IEP.01</t>
+  </si>
+  <si>
+    <t>PR.LAT.IEP.02</t>
+  </si>
+  <si>
+    <t>PR.LAT.23.</t>
+  </si>
+  <si>
+    <t>Spēles kārta</t>
+  </si>
+  <si>
+    <t>KAR</t>
+  </si>
+  <si>
+    <t>PR.LAT.KAR.01</t>
+  </si>
+  <si>
+    <t>PR.LAT.KAR.02</t>
+  </si>
+  <si>
+    <t>PR.LAT.24.</t>
+  </si>
+  <si>
+    <t>Spēles līdera tabula</t>
+  </si>
+  <si>
+    <t>PR.LAT.LID.02</t>
+  </si>
+  <si>
+    <t>Spēles otrā lietotāja otrā kārta</t>
+  </si>
+  <si>
+    <t>Spēles AI kārta</t>
+  </si>
+  <si>
+    <t>Spēles līdera tabula saglabāšana 1 pret 1</t>
+  </si>
+  <si>
+    <t>Spēles līdera tabula saglabāšana AI</t>
+  </si>
+  <si>
+    <t>Spēles saglabāšana ar AI veidu</t>
+  </si>
+  <si>
+    <t>Spēles saglabāšana ar 1 pret 1 veidu</t>
+  </si>
+  <si>
+    <t>Spēles iepriekšējais progress ar AI veidu</t>
+  </si>
+  <si>
+    <t>Spēles iepriekšējais progress ar 1 pret 1 veidu</t>
+  </si>
+  <si>
+    <t>1)Jābūt izvēlētai spēlet ar botu
+2)Lietotājam sākuma ir jāizdara gaita, jāuzbrūk, lai nav tukša teritorija
+3)Lietotājam ir jānospiež "OK" poga pēc izdarītā gaita.</t>
+  </si>
+  <si>
+    <t>Pēc lietotāja izdarītas gaitas AI mobilizēs savā vājāka vietā no 1 līdz 2 rotas skaitu</t>
+  </si>
+  <si>
+    <t>1)AI saņem informāciju, ka ir jādara AIKustiba, kur prioritāte ir LSPRUzbrukums();
 2)LSPRUzbrukums(), dabū State, no kura tiks darītas gaitas
 3)Tagad meklē ar distance &lt; 1.96f, tuvākās lietotāja teritorijas, kur stateControllerrotasSkaitsByPlayer[Valstis.Speletaji.PLAYER] &lt; objekti.noKuraStateLSPRKontrole.rotasSkaitsByPlayer[Valstis.Speletaji.LSPR]
 4)Ja ir atrasts UzbruksanasState, tad uzbrūk lietotājam un ieņem teritoriju.
@@ -1149,107 +1341,10 @@
 7)Ar otru ciklu izdzēšs ārā vecās LSPR(AI) rotas teritorijā</t>
   </si>
   <si>
-    <t>PR.LAT.20.</t>
-  </si>
-  <si>
-    <t>PR.LAT.21.</t>
-  </si>
-  <si>
-    <t>PR.LAT.22.</t>
-  </si>
-  <si>
-    <t>Spēles AI uzbrukšana</t>
-  </si>
-  <si>
-    <t>Spēles AI mobilizēšana</t>
-  </si>
-  <si>
-    <t>Spēles AI atkāpšanās</t>
-  </si>
-  <si>
-    <t>1)Funkcija pārbaudīs, ja objekti.rotuSkaitsIzv &lt; StateController.rotasSkaitsByPlayer[Valsts.Speletaji.LSPR, tad irZaudets = true
-6)Parādīsies ziņojums, ka ir zaudējis cīņu</t>
-  </si>
-  <si>
-    <t>TZ.B.15.</t>
-  </si>
-  <si>
-    <t>TZ.B.16.</t>
-  </si>
-  <si>
-    <t>TZ.B.17.</t>
-  </si>
-  <si>
-    <t>TZ.B.18.</t>
-  </si>
-  <si>
-    <t>TZ.B.19.</t>
-  </si>
-  <si>
-    <t>TZ.B.20.</t>
-  </si>
-  <si>
-    <t>TZ.B.21.</t>
-  </si>
-  <si>
-    <t>TZ.B.22.</t>
-  </si>
-  <si>
-    <t>TZ.B.23.</t>
-  </si>
-  <si>
-    <t>TZ.B.24.</t>
-  </si>
-  <si>
-    <t>TZ.B.25.</t>
-  </si>
-  <si>
-    <t>TZ.B.26.</t>
-  </si>
-  <si>
-    <t>TZ.B.27.</t>
-  </si>
-  <si>
-    <t>TZ.B.28.</t>
-  </si>
-  <si>
-    <t>TZ.B.29.</t>
-  </si>
-  <si>
-    <t>TZ.B.30.</t>
-  </si>
-  <si>
-    <t>TZ.B.31.</t>
-  </si>
-  <si>
-    <t>TZ.B.32.</t>
-  </si>
-  <si>
-    <t>TZ.B.33.</t>
-  </si>
-  <si>
-    <t>TZ.B.34.</t>
-  </si>
-  <si>
-    <t>TZ.W.1.</t>
-  </si>
-  <si>
-    <t>TZ.W.2.</t>
-  </si>
-  <si>
-    <t>TZ.W.3.</t>
-  </si>
-  <si>
-    <t>TZ.W.4.</t>
-  </si>
-  <si>
-    <t>TZ.W.5.</t>
-  </si>
-  <si>
-    <t>TZ.W.6.</t>
-  </si>
-  <si>
-    <t>TZ.W.7.</t>
+    <t>1)AI saņem informāciju, ka ir jādara AIKustiba, kur prioritāte ir LSPRUzbrukums();
+2)Kad saprot, kad nevar uzbrukt nekur, jo objekti.uzbruksanasState == null, tad pāriet uz mobilizēšanu metodi, kur izsauc metodi noKuraStateLSPRGajiens();
+3)
+4)</t>
   </si>
 </sst>
 </file>
@@ -1467,11 +1562,11 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1789,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19930E9-390E-44F3-A281-41A941A5DA96}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:C36"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,30 +2189,16 @@
       <c r="C35" s="16"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="16"/>
+      <c r="A36" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>408</v>
+      </c>
       <c r="C36" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B11:C11"/>
@@ -2132,6 +2213,24 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2140,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E44EBC5-0971-4FC8-9842-6658A0759BB0}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,26 +2537,42 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B38" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B39" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B40" t="s">
-        <v>368</v>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>407</v>
+      </c>
+      <c r="B41" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>412</v>
+      </c>
+      <c r="B42" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -2470,10 +2585,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214DAA82-A5B2-4DC9-AAA1-ECC0BC576048}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:B58"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3451,19 +3566,19 @@
       <c r="A47" t="s">
         <v>317</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="10" t="s">
         <v>312</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="10" t="s">
         <v>320</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="F47" s="25" t="s">
+      <c r="F47" s="10" t="s">
         <v>322</v>
       </c>
       <c r="G47" s="10" t="s">
@@ -3489,22 +3604,22 @@
       <c r="A49" t="s">
         <v>329</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="E49" s="10" t="s">
         <v>338</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="G49" s="10" t="s">
         <v>341</v>
       </c>
       <c r="H49" t="s">
@@ -3515,22 +3630,22 @@
       <c r="A50" t="s">
         <v>330</v>
       </c>
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D50" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="E50" s="25" t="s">
+      <c r="E50" s="10" t="s">
         <v>339</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="25" t="s">
+      <c r="G50" s="10" t="s">
         <v>342</v>
       </c>
       <c r="H50" t="s">
@@ -3541,22 +3656,22 @@
       <c r="A51" t="s">
         <v>333</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="D51" s="25" t="s">
+      <c r="D51" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E51" s="25" t="s">
+      <c r="E51" s="10" t="s">
         <v>340</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G51" s="25" t="s">
+      <c r="G51" s="10" t="s">
         <v>343</v>
       </c>
       <c r="H51" t="s">
@@ -3577,22 +3692,22 @@
       <c r="A53" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="10" t="s">
         <v>344</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="D53" s="25" t="s">
+      <c r="D53" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="10" t="s">
         <v>345</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G53" s="25" t="s">
+      <c r="G53" s="10" t="s">
         <v>347</v>
       </c>
       <c r="H53" t="s">
@@ -3603,23 +3718,23 @@
       <c r="A54" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="10" t="s">
         <v>346</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="D54" s="25" t="s">
+      <c r="D54" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="E54" s="25" t="s">
+      <c r="E54" s="10" t="s">
         <v>345</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G54" s="25" t="s">
-        <v>369</v>
+      <c r="G54" s="10" t="s">
+        <v>367</v>
       </c>
       <c r="H54" t="s">
         <v>204</v>
@@ -3639,22 +3754,22 @@
       <c r="A56" t="s">
         <v>230</v>
       </c>
-      <c r="B56" s="25" t="s">
+      <c r="B56" s="10" t="s">
         <v>348</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="D56" s="25" t="s">
+      <c r="D56" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="E56" s="25" t="s">
+      <c r="E56" s="10" t="s">
         <v>345</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G56" s="25" t="s">
+      <c r="G56" s="10" t="s">
         <v>355</v>
       </c>
       <c r="H56" t="s">
@@ -3673,43 +3788,232 @@
     </row>
     <row r="58" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>398</v>
+      </c>
+      <c r="B58" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="C58" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="E58" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="D58" s="25" t="s">
-        <v>358</v>
-      </c>
-      <c r="E58" s="25" t="s">
+      <c r="F58" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="F58" s="25" t="s">
+      <c r="G58" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="H58" t="s">
         <v>361</v>
       </c>
-      <c r="G58" s="10" t="s">
+    </row>
+    <row r="59" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>399</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H59" t="s">
         <v>362</v>
       </c>
-      <c r="H58" t="s">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>400</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="H60" t="s">
         <v>363</v>
       </c>
     </row>
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>401</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="H61" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="23"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+    </row>
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>410</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>415</v>
+      </c>
+      <c r="H63" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>411</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>416</v>
+      </c>
+      <c r="H64" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
+    </row>
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>402</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="H66" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>414</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="H67" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="23"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+    </row>
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>403</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="H69" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>404</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="H70" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="15"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+    </row>
+    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>405</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="H72" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>406</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="H73" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A18:H18"/>
+  <mergeCells count="17">
+    <mergeCell ref="A65:H65"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="A68:H68"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A29:H29"/>
     <mergeCell ref="A34:H34"/>
@@ -3723,8 +4027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80724A93-B008-4A33-8DA6-F5EB9092A099}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,16 +4070,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4190,7 +4494,7 @@
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B28" s="11">
         <v>45447</v>
@@ -4210,7 +4514,7 @@
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B29" s="11">
         <v>45447</v>
@@ -4240,7 +4544,7 @@
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B31" s="11">
         <v>45447</v>
@@ -4260,7 +4564,7 @@
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B32" s="11">
         <v>45447</v>
@@ -4280,7 +4584,7 @@
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B33" s="11">
         <v>45447</v>
@@ -4300,7 +4604,7 @@
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B34" s="11">
         <v>45447</v>
@@ -4330,7 +4634,7 @@
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B36" s="11">
         <v>45447</v>
@@ -4350,7 +4654,7 @@
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B37" s="11">
         <v>45447</v>
@@ -4370,7 +4674,7 @@
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B38" s="11">
         <v>45447</v>
@@ -4390,7 +4694,7 @@
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B39" s="11">
         <v>45447</v>
@@ -4420,7 +4724,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B41" s="11">
         <v>45447</v>
@@ -4440,7 +4744,7 @@
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B42" s="11">
         <v>45447</v>
@@ -4460,7 +4764,7 @@
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B43" s="11">
         <v>45447</v>
@@ -4480,7 +4784,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B44" s="11">
         <v>45447</v>
@@ -4500,7 +4804,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B45" s="11">
         <v>45447</v>
@@ -4520,7 +4824,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B46" s="11">
         <v>45447</v>
@@ -4550,7 +4854,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B48" s="11">
         <v>45447</v>
@@ -4580,7 +4884,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B50" s="11">
         <v>45447</v>
@@ -4600,7 +4904,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B51" s="11">
         <v>45447</v>
@@ -4630,7 +4934,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B53" s="11">
         <v>45447</v>
@@ -4638,7 +4942,7 @@
       <c r="C53" t="s">
         <v>317</v>
       </c>
-      <c r="D53" s="25" t="s">
+      <c r="D53" s="10" t="s">
         <v>312</v>
       </c>
       <c r="E53" t="s">
@@ -4649,20 +4953,20 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B55" s="11">
         <v>45447</v>
@@ -4670,7 +4974,7 @@
       <c r="C55" t="s">
         <v>329</v>
       </c>
-      <c r="D55" s="25" t="s">
+      <c r="D55" s="10" t="s">
         <v>331</v>
       </c>
       <c r="E55" t="s">
@@ -4682,7 +4986,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B56" s="11">
         <v>45447</v>
@@ -4690,7 +4994,7 @@
       <c r="C56" t="s">
         <v>330</v>
       </c>
-      <c r="D56" s="25" t="s">
+      <c r="D56" s="10" t="s">
         <v>332</v>
       </c>
       <c r="E56" t="s">
@@ -4702,7 +5006,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B57" s="11">
         <v>45447</v>
@@ -4710,7 +5014,7 @@
       <c r="C57" t="s">
         <v>333</v>
       </c>
-      <c r="D57" s="25" t="s">
+      <c r="D57" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E57" t="s">
@@ -4732,7 +5036,7 @@
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B59" s="11">
         <v>45447</v>
@@ -4740,7 +5044,7 @@
       <c r="C59" t="s">
         <v>137</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D59" s="10" t="s">
         <v>344</v>
       </c>
       <c r="E59" t="s">
@@ -4752,7 +5056,7 @@
     </row>
     <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B60" s="11">
         <v>45447</v>
@@ -4760,7 +5064,7 @@
       <c r="C60" t="s">
         <v>144</v>
       </c>
-      <c r="D60" s="25" t="s">
+      <c r="D60" s="10" t="s">
         <v>346</v>
       </c>
       <c r="E60" t="s">
@@ -4782,7 +5086,7 @@
     </row>
     <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B62" s="11">
         <v>45447</v>
@@ -4790,7 +5094,7 @@
       <c r="C62" t="s">
         <v>230</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="D62" s="10" t="s">
         <v>348</v>
       </c>
       <c r="E62" t="s">
@@ -4812,16 +5116,16 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B64" s="11">
         <v>45447</v>
       </c>
       <c r="C64" t="s">
+        <v>398</v>
+      </c>
+      <c r="D64" s="10" t="s">
         <v>356</v>
-      </c>
-      <c r="D64" s="25" t="s">
-        <v>357</v>
       </c>
       <c r="E64" t="s">
         <v>81</v>
@@ -4832,16 +5136,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A52:H52"/>
-    <mergeCell ref="A54:H54"/>
-    <mergeCell ref="A58:H58"/>
-    <mergeCell ref="A61:H61"/>
-    <mergeCell ref="A63:H63"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="A49:H49"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A2:H2"/>
@@ -4854,6 +5148,16 @@
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A52:H52"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="A58:H58"/>
+    <mergeCell ref="A61:H61"/>
+    <mergeCell ref="A63:H63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>